<commit_message>
remove empty spaces in 'Locality'
</commit_message>
<xml_diff>
--- a/data/Legislative.xlsx
+++ b/data/Legislative.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -56,9 +56,6 @@
     <t>WU16</t>
   </si>
   <si>
-    <t xml:space="preserve">Wiejce </t>
-  </si>
-  <si>
     <t>WU53</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Wiejce</t>
   </si>
   <si>
-    <t xml:space="preserve">Czelin </t>
-  </si>
-  <si>
     <t>Daleszyce</t>
   </si>
   <si>
@@ -129,12 +123,6 @@
   </si>
   <si>
     <t>Słopiec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Świnoujście </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woźniki </t>
   </si>
   <si>
     <t>Mirów</t>
@@ -1355,39 +1343,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1416,10 +1404,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1448,10 +1436,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -1480,10 +1468,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -1512,10 +1500,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -1544,10 +1532,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -1576,10 +1564,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1608,10 +1596,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1640,10 +1628,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1672,10 +1660,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -1704,10 +1692,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -1736,10 +1724,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -1768,10 +1756,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1800,10 +1788,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1832,10 +1820,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1864,10 +1852,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1896,10 +1884,10 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1911,10 +1899,10 @@
         <v>151</v>
       </c>
       <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
         <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
       </c>
       <c r="H18">
         <v>52.64</v>
@@ -1928,10 +1916,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -1943,10 +1931,10 @@
         <v>200</v>
       </c>
       <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
         <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>16</v>
       </c>
       <c r="H19">
         <v>53.85</v>
@@ -1960,10 +1948,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
@@ -1992,10 +1980,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -2024,10 +2012,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -2039,10 +2027,10 @@
         <v>147</v>
       </c>
       <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
         <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
       </c>
       <c r="H22">
         <v>52.64</v>
@@ -2056,10 +2044,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -2071,10 +2059,10 @@
         <v>166</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23">
         <v>50.85</v>
@@ -2088,10 +2076,10 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -2103,10 +2091,10 @@
         <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H24">
         <v>50.85</v>
@@ -2120,10 +2108,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -2135,10 +2123,10 @@
         <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25">
         <v>50.85</v>
@@ -2152,10 +2140,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -2167,10 +2155,10 @@
         <v>145</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H26">
         <v>50.85</v>
@@ -2184,10 +2172,10 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -2199,10 +2187,10 @@
         <v>177</v>
       </c>
       <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
         <v>15</v>
-      </c>
-      <c r="G27" t="s">
-        <v>16</v>
       </c>
       <c r="H27">
         <v>53.85</v>
@@ -2216,10 +2204,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -2231,10 +2219,10 @@
         <v>177</v>
       </c>
       <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
         <v>15</v>
-      </c>
-      <c r="G28" t="s">
-        <v>16</v>
       </c>
       <c r="H28">
         <v>53.85</v>
@@ -2248,10 +2236,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -2263,10 +2251,10 @@
         <v>177</v>
       </c>
       <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
         <v>15</v>
-      </c>
-      <c r="G29" t="s">
-        <v>16</v>
       </c>
       <c r="H29">
         <v>53.85</v>
@@ -2280,10 +2268,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
@@ -2295,10 +2283,10 @@
         <v>177</v>
       </c>
       <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
         <v>15</v>
-      </c>
-      <c r="G30" t="s">
-        <v>16</v>
       </c>
       <c r="H30">
         <v>53.85</v>
@@ -2312,10 +2300,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -2327,10 +2315,10 @@
         <v>177</v>
       </c>
       <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
         <v>15</v>
-      </c>
-      <c r="G31" t="s">
-        <v>16</v>
       </c>
       <c r="H31">
         <v>53.85</v>
@@ -2344,10 +2332,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -2359,10 +2347,10 @@
         <v>177</v>
       </c>
       <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
         <v>15</v>
-      </c>
-      <c r="G32" t="s">
-        <v>16</v>
       </c>
       <c r="H32">
         <v>53.85</v>
@@ -2376,10 +2364,10 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
@@ -2391,10 +2379,10 @@
         <v>177</v>
       </c>
       <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
         <v>15</v>
-      </c>
-      <c r="G33" t="s">
-        <v>16</v>
       </c>
       <c r="H33">
         <v>53.85</v>
@@ -2408,10 +2396,10 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -2423,10 +2411,10 @@
         <v>177</v>
       </c>
       <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
         <v>15</v>
-      </c>
-      <c r="G34" t="s">
-        <v>16</v>
       </c>
       <c r="H34">
         <v>53.85</v>
@@ -2440,10 +2428,10 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -2455,10 +2443,10 @@
         <v>186</v>
       </c>
       <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
         <v>18</v>
-      </c>
-      <c r="G35" t="s">
-        <v>19</v>
       </c>
       <c r="H35">
         <v>54.13</v>
@@ -2472,10 +2460,10 @@
     </row>
     <row r="36" spans="1:12">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -2487,10 +2475,10 @@
         <v>187</v>
       </c>
       <c r="F36" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" t="s">
         <v>18</v>
-      </c>
-      <c r="G36" t="s">
-        <v>19</v>
       </c>
       <c r="H36">
         <v>54.13</v>
@@ -2504,10 +2492,10 @@
     </row>
     <row r="37" spans="1:12">
       <c r="A37" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
@@ -2519,10 +2507,10 @@
         <v>169</v>
       </c>
       <c r="F37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" t="s">
         <v>20</v>
-      </c>
-      <c r="G37" t="s">
-        <v>21</v>
       </c>
       <c r="H37">
         <v>49.44</v>
@@ -2536,10 +2524,10 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -2551,10 +2539,10 @@
         <v>187</v>
       </c>
       <c r="F38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" t="s">
         <v>18</v>
-      </c>
-      <c r="G38" t="s">
-        <v>19</v>
       </c>
       <c r="H38">
         <v>54.13</v>
@@ -2568,10 +2556,10 @@
     </row>
     <row r="39" spans="1:12">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -2583,10 +2571,10 @@
         <v>204</v>
       </c>
       <c r="F39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" t="s">
         <v>22</v>
-      </c>
-      <c r="G39" t="s">
-        <v>23</v>
       </c>
       <c r="H39">
         <v>48.15</v>
@@ -2600,10 +2588,10 @@
     </row>
     <row r="40" spans="1:12">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
         <v>3</v>
@@ -2615,10 +2603,10 @@
         <v>158</v>
       </c>
       <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
         <v>24</v>
-      </c>
-      <c r="G40" t="s">
-        <v>25</v>
       </c>
       <c r="H40">
         <v>52.24</v>
@@ -2632,10 +2620,10 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
         <v>3</v>
@@ -2647,10 +2635,10 @@
         <v>242</v>
       </c>
       <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
         <v>24</v>
-      </c>
-      <c r="G41" t="s">
-        <v>25</v>
       </c>
       <c r="H41">
         <v>52.24</v>
@@ -2664,10 +2652,10 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -2679,10 +2667,10 @@
         <v>147</v>
       </c>
       <c r="F42" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" t="s">
         <v>13</v>
-      </c>
-      <c r="G42" t="s">
-        <v>14</v>
       </c>
       <c r="H42">
         <v>52.64</v>
@@ -2696,10 +2684,10 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -2711,10 +2699,10 @@
         <v>176</v>
       </c>
       <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
         <v>15</v>
-      </c>
-      <c r="G43" t="s">
-        <v>16</v>
       </c>
       <c r="H43">
         <v>53.85</v>
@@ -2728,10 +2716,10 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -2791,39 +2779,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -2852,10 +2840,10 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -2884,10 +2872,10 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -2916,10 +2904,10 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -2948,10 +2936,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -2980,10 +2968,10 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -2995,10 +2983,10 @@
         <v>167</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <v>52.64</v>
@@ -3012,10 +3000,10 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -3044,10 +3032,10 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -3059,7 +3047,7 @@
         <v>172</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -3076,10 +3064,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -3108,10 +3096,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
@@ -3123,7 +3111,7 @@
         <v>168</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -3140,10 +3128,10 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -3172,10 +3160,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
@@ -3187,7 +3175,7 @@
         <v>168</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -3204,10 +3192,10 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -3236,10 +3224,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -3268,10 +3256,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -3283,10 +3271,10 @@
         <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16">
         <v>52.64</v>
@@ -3300,10 +3288,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -3315,10 +3303,10 @@
         <v>149</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H17">
         <v>50.79</v>
@@ -3332,10 +3320,10 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -3347,10 +3335,10 @@
         <v>211</v>
       </c>
       <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
         <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
       </c>
       <c r="H18">
         <v>48.15</v>
@@ -3364,10 +3352,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -3379,10 +3367,10 @@
         <v>172</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19">
         <v>50.85</v>
@@ -3396,10 +3384,10 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -3411,10 +3399,10 @@
         <v>172</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20">
         <v>50.85</v>
@@ -3428,10 +3416,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
@@ -3443,10 +3431,10 @@
         <v>211</v>
       </c>
       <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" t="s">
         <v>22</v>
-      </c>
-      <c r="G21" t="s">
-        <v>23</v>
       </c>
       <c r="H21">
         <v>48.15</v>
@@ -3460,10 +3448,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
@@ -3475,10 +3463,10 @@
         <v>177</v>
       </c>
       <c r="F22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H22">
         <v>53.29</v>
@@ -3492,10 +3480,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
@@ -3507,10 +3495,10 @@
         <v>181</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H23">
         <v>52.92</v>
@@ -3524,10 +3512,10 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -3539,10 +3527,10 @@
         <v>251</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24">
         <v>49.44</v>
@@ -3556,10 +3544,10 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
@@ -3571,10 +3559,10 @@
         <v>177</v>
       </c>
       <c r="F25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H25">
         <v>53.29</v>
@@ -3588,10 +3576,10 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
@@ -3603,10 +3591,10 @@
         <v>246</v>
       </c>
       <c r="F26" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
       </c>
       <c r="H26">
         <v>54.13</v>
@@ -3620,10 +3608,10 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
@@ -3635,10 +3623,10 @@
         <v>168</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H27">
         <v>50.43</v>
@@ -3652,10 +3640,10 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -3667,10 +3655,10 @@
         <v>213</v>
       </c>
       <c r="F28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G28" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H28">
         <v>50.77</v>
@@ -3684,10 +3672,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
@@ -3699,10 +3687,10 @@
         <v>197</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H29">
         <v>50.43</v>
@@ -3716,10 +3704,10 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
@@ -3731,10 +3719,10 @@
         <v>197</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H30">
         <v>50.43</v>
@@ -3748,10 +3736,10 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
@@ -3763,10 +3751,10 @@
         <v>197</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H31">
         <v>50.43</v>
@@ -3780,10 +3768,10 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -3795,10 +3783,10 @@
         <v>183</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H32">
         <v>53.85</v>
@@ -3812,10 +3800,10 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -3827,10 +3815,10 @@
         <v>183</v>
       </c>
       <c r="F33" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33">
         <v>53.85</v>
@@ -3844,10 +3832,10 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
@@ -3859,10 +3847,10 @@
         <v>183</v>
       </c>
       <c r="F34" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34">
         <v>53.85</v>
@@ -3876,10 +3864,10 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -3891,10 +3879,10 @@
         <v>183</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35">
         <v>53.85</v>
@@ -3908,10 +3896,10 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -3923,10 +3911,10 @@
         <v>183</v>
       </c>
       <c r="F36" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36">
         <v>53.85</v>
@@ -3940,10 +3928,10 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
@@ -3955,10 +3943,10 @@
         <v>183</v>
       </c>
       <c r="F37" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H37">
         <v>53.85</v>
@@ -3972,10 +3960,10 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s">
         <v>3</v>
@@ -3987,10 +3975,10 @@
         <v>150</v>
       </c>
       <c r="F38" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H38">
         <v>52.24</v>
@@ -4004,10 +3992,10 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
         <v>3</v>
@@ -4019,10 +4007,10 @@
         <v>223</v>
       </c>
       <c r="F39" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H39">
         <v>52.24</v>
@@ -4036,10 +4024,10 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
         <v>10</v>
@@ -4051,10 +4039,10 @@
         <v>160</v>
       </c>
       <c r="F40" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H40">
         <v>52.24</v>
@@ -4068,10 +4056,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
         <v>10</v>
@@ -4083,10 +4071,10 @@
         <v>187</v>
       </c>
       <c r="F41" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H41">
         <v>52.24</v>
@@ -4100,10 +4088,10 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
@@ -4115,10 +4103,10 @@
         <v>151</v>
       </c>
       <c r="F42" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H42">
         <v>52.24</v>
@@ -4132,10 +4120,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>3</v>
@@ -4147,10 +4135,10 @@
         <v>147</v>
       </c>
       <c r="F43" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="G43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H43">
         <v>52.24</v>
@@ -4164,10 +4152,10 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
         <v>3</v>
@@ -4179,10 +4167,10 @@
         <v>148</v>
       </c>
       <c r="F44" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G44" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H44">
         <v>50.62</v>
@@ -4196,10 +4184,10 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
@@ -4211,10 +4199,10 @@
         <v>246</v>
       </c>
       <c r="F45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H45">
         <v>49.44</v>
@@ -4228,10 +4216,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
@@ -4243,10 +4231,10 @@
         <v>198</v>
       </c>
       <c r="F46" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H46">
         <v>52.56</v>
@@ -4260,10 +4248,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
@@ -4275,10 +4263,10 @@
         <v>230</v>
       </c>
       <c r="F47" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H47">
         <v>51.27</v>
@@ -4292,10 +4280,10 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
@@ -4307,10 +4295,10 @@
         <v>221</v>
       </c>
       <c r="F48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G48" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H48">
         <v>52.45</v>
@@ -4324,10 +4312,10 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -4339,10 +4327,10 @@
         <v>230</v>
       </c>
       <c r="F49" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H49">
         <v>53.76</v>
@@ -4356,10 +4344,10 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -4371,10 +4359,10 @@
         <v>269</v>
       </c>
       <c r="F50" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H50">
         <v>50.43</v>
@@ -4388,10 +4376,10 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C51" t="s">
         <v>3</v>
@@ -4403,10 +4391,10 @@
         <v>269</v>
       </c>
       <c r="F51" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G51" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H51">
         <v>50.43</v>
@@ -4420,10 +4408,10 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
@@ -4435,10 +4423,10 @@
         <v>269</v>
       </c>
       <c r="F52" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G52" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H52">
         <v>50.43</v>
@@ -4452,10 +4440,10 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C53" t="s">
         <v>3</v>
@@ -4467,10 +4455,10 @@
         <v>269</v>
       </c>
       <c r="F53" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H53">
         <v>50.43</v>

</xml_diff>